<commit_message>
minor changes to the schedule and show flyer
minor changes to the schedule and show flyer; added Kathy and Laura Hull bio to cast list page
</commit_message>
<xml_diff>
--- a/howTo26/How2$ production.xlsx
+++ b/howTo26/How2$ production.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Seagate X/RVCOprod/website/howTo26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEA9F0-28B7-F042-A52D-FE7D489C4336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4E6FEE-4BDF-8A40-86C1-D6D13F0AA2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="600" windowWidth="27860" windowHeight="20600" activeTab="1" xr2:uid="{E38B6315-D279-724B-88A4-0AE2C1BF2347}"/>
+    <workbookView xWindow="4040" yWindow="600" windowWidth="27860" windowHeight="20600" activeTab="1" xr2:uid="{E38B6315-D279-724B-88A4-0AE2C1BF2347}"/>
   </bookViews>
   <sheets>
     <sheet name="Cast" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
   <si>
     <t xml:space="preserve">EMERGENCY CONTACT </t>
   </si>
@@ -375,15 +375,6 @@
     <t>Act I</t>
   </si>
   <si>
-    <t>() delineates curtain placement</t>
-  </si>
-  <si>
-    <t>!  delineates very short turnaround time</t>
-  </si>
-  <si>
-    <t>* repeat scenes</t>
-  </si>
-  <si>
     <t>In front of the traveler</t>
   </si>
   <si>
@@ -607,13 +598,6 @@
   </si>
   <si>
     <t>Office is stage right in front of Biggley's office.  Desk &amp; chair</t>
-  </si>
-  <si>
-    <t>Moving wall oppossite mailroom wall
-Some guys are watching in the boardroom. May need an old TV.</t>
-  </si>
-  <si>
-    <t>Chorus 'cleaning up'</t>
   </si>
   <si>
     <r>
@@ -760,6 +744,13 @@
   </si>
   <si>
     <t>Secretary, Wickette girl</t>
+  </si>
+  <si>
+    <t>Moving wall oppossite mailroom wall.
+Some guys are watching in the boardroom or not. May need an old TV.</t>
+  </si>
+  <si>
+    <t>Scrubwomen 'cleaning up'</t>
   </si>
 </sst>
 </file>
@@ -1884,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H21" s="25">
         <v>19</v>
@@ -1910,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H22" s="25">
         <v>20</v>
@@ -1952,7 +1943,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="9"/>
       <c r="G24" s="10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H24" s="25">
         <v>22</v>
@@ -1978,7 +1969,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H25" s="25">
         <v>24</v>
@@ -2004,7 +1995,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H26" s="25">
         <v>25</v>
@@ -2188,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FED2AE-CC40-A149-B7C9-8B9701A2964F}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2207,25 +2198,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="31" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B1" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>133</v>
-      </c>
       <c r="E1" s="33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2243,16 +2234,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="47" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2264,16 +2255,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E4" s="48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2285,13 +2276,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2303,59 +2294,59 @@
         <v>22</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="B7" s="43" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C7" s="43">
         <v>22</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E7" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="42" t="s">
         <v>142</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="B8" s="43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C8" s="43">
         <v>23</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H8" s="51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2364,13 +2355,16 @@
         <v>33</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E9" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>181</v>
+        <v>178</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>186</v>
       </c>
       <c r="H9" s="46"/>
     </row>
@@ -2383,13 +2377,13 @@
         <v>38</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="43">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2398,19 +2392,17 @@
         <v>40</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E11" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>191</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="G11" s="54"/>
       <c r="H11" s="46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2422,16 +2414,16 @@
         <v>45</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E12" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H12" s="51" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2443,16 +2435,16 @@
         <v>56</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E13" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H13" s="51" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2464,16 +2456,16 @@
         <v>64</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G14" s="56" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.2">
@@ -2485,16 +2477,16 @@
         <v>68</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E15" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G15" s="55" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2506,19 +2498,19 @@
         <v>69</v>
       </c>
       <c r="D16" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="G16" s="38" t="s">
-        <v>161</v>
-      </c>
       <c r="H16" s="46" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2530,16 +2522,16 @@
         <v>72</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2551,13 +2543,13 @@
         <v>76</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2569,16 +2561,16 @@
         <v>79</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -2595,7 +2587,7 @@
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B22" s="43">
         <v>1</v>
@@ -2604,16 +2596,16 @@
         <v>93</v>
       </c>
       <c r="D22" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E22" s="48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H22" s="52" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2625,16 +2617,16 @@
         <v>99</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E23" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H23" s="46" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2646,13 +2638,13 @@
         <v>105</v>
       </c>
       <c r="D24" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="46" t="s">
         <v>164</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="H24" s="46" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="47" customFormat="1" ht="28" x14ac:dyDescent="0.2">
@@ -2664,17 +2656,17 @@
         <v>111</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E25" s="48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="47" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H25" s="53" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2686,20 +2678,20 @@
         <v>115</v>
       </c>
       <c r="D26" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="40" t="s">
-        <v>172</v>
-      </c>
       <c r="G26" s="40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H26" s="40"/>
     </row>
-    <row r="27" spans="1:8" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="47" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="B27" s="43">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2708,19 +2700,19 @@
         <v>125</v>
       </c>
       <c r="D27" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>173</v>
-      </c>
       <c r="G27" s="40" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -2732,16 +2724,16 @@
         <v>128</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H28" s="46" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -2753,13 +2745,13 @@
         <v>133</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E29" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -2771,30 +2763,30 @@
         <v>134</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E30" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H30" s="46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B31" s="43" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C31" s="43">
         <v>143</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E31" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H31" s="46"/>
     </row>
@@ -2807,16 +2799,16 @@
         <v>143</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E32" s="45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H32" s="54" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
@@ -2829,22 +2821,16 @@
       <c r="D34" s="40"/>
       <c r="E34" s="43"/>
     </row>
-    <row r="35" spans="2:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="D35" s="44" t="s">
-        <v>106</v>
-      </c>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="44"/>
       <c r="E35" s="45"/>
     </row>
-    <row r="36" spans="2:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="D36" s="44" t="s">
-        <v>107</v>
-      </c>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="44"/>
       <c r="E36" s="45"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D37" s="44" t="s">
-        <v>108</v>
-      </c>
+      <c r="D37" s="44"/>
       <c r="E37" s="45"/>
     </row>
   </sheetData>

</xml_diff>